<commit_message>
chore: adiciona todos os arquivos do dashboard
</commit_message>
<xml_diff>
--- a/Planilhas/Carga.xlsx
+++ b/Planilhas/Carga.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariocabral/Desktop/MeuDashboard/Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CCF09F-0296-BE44-8D04-D34DCFB33095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85886F43-65D6-1347-ADA4-6DC9771ACC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="37420" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="37420" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acessos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="199">
   <si>
     <t>UsuarioID</t>
   </si>
@@ -552,6 +552,90 @@
   </si>
   <si>
     <t>DataCadastro</t>
+  </si>
+  <si>
+    <t>StatusModulo</t>
+  </si>
+  <si>
+    <t>TempoAcessoModuloEmHoras</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <t>0:00:01</t>
+  </si>
+  <si>
+    <t>0:02:44</t>
+  </si>
+  <si>
+    <t>0:00:39</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>0:00:59</t>
+  </si>
+  <si>
+    <t>Expirado (Não Realizado)</t>
+  </si>
+  <si>
+    <t>0:00:00</t>
+  </si>
+  <si>
+    <t>Reprovado</t>
+  </si>
+  <si>
+    <t>0:00:21</t>
+  </si>
+  <si>
+    <t>0:00:19</t>
+  </si>
+  <si>
+    <t>0:00:18</t>
+  </si>
+  <si>
+    <t>0:00:38</t>
+  </si>
+  <si>
+    <t>0:00:30</t>
+  </si>
+  <si>
+    <t>0:00:03</t>
+  </si>
+  <si>
+    <t>0:01:06</t>
+  </si>
+  <si>
+    <t>0:01:30</t>
+  </si>
+  <si>
+    <t>0:00:15</t>
+  </si>
+  <si>
+    <t>0:00:40</t>
+  </si>
+  <si>
+    <t>Não Iniciado</t>
+  </si>
+  <si>
+    <t>0:00:02</t>
+  </si>
+  <si>
+    <t>0:00:26</t>
+  </si>
+  <si>
+    <t>0:19:23</t>
+  </si>
+  <si>
+    <t>0:00:10</t>
+  </si>
+  <si>
+    <t>0:02:48</t>
+  </si>
+  <si>
+    <t>0:20:31</t>
   </si>
 </sst>
 </file>
@@ -930,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2444,10 +2528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DEF9A41-F379-1F49-B5CE-AAD7CB2EE5A6}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2463,7 +2547,7 @@
     <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2491,8 +2575,14 @@
       <c r="I1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1421046</v>
       </c>
@@ -2521,8 +2611,14 @@
         <f>VLOOKUP(A2,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1421046</v>
       </c>
@@ -2551,8 +2647,14 @@
         <f>VLOOKUP(A3,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1421046</v>
       </c>
@@ -2581,8 +2683,14 @@
         <f>VLOOKUP(A4,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>173</v>
+      </c>
+      <c r="K4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1421046</v>
       </c>
@@ -2608,8 +2716,14 @@
         <f>VLOOKUP(A5,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1421046</v>
       </c>
@@ -2632,8 +2746,14 @@
         <f>VLOOKUP(A6,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>179</v>
+      </c>
+      <c r="K6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1421046</v>
       </c>
@@ -2656,8 +2776,14 @@
         <f>VLOOKUP(A7,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1421046</v>
       </c>
@@ -2680,8 +2806,14 @@
         <f>VLOOKUP(A8,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>179</v>
+      </c>
+      <c r="K8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1421046</v>
       </c>
@@ -2707,8 +2839,14 @@
         <f>VLOOKUP(A9,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1421046</v>
       </c>
@@ -2734,8 +2872,14 @@
         <f>VLOOKUP(A10,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>179</v>
+      </c>
+      <c r="K10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1421046</v>
       </c>
@@ -2764,8 +2908,14 @@
         <f>VLOOKUP(A11,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>181</v>
+      </c>
+      <c r="K11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1421046</v>
       </c>
@@ -2794,8 +2944,14 @@
         <f>VLOOKUP(A12,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>181</v>
+      </c>
+      <c r="K12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1421046</v>
       </c>
@@ -2824,8 +2980,14 @@
         <f>VLOOKUP(A13,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>181</v>
+      </c>
+      <c r="K13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1421046</v>
       </c>
@@ -2854,8 +3016,14 @@
         <f>VLOOKUP(A14,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1421046</v>
       </c>
@@ -2884,8 +3052,14 @@
         <f>VLOOKUP(A15,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>181</v>
+      </c>
+      <c r="K15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1421046</v>
       </c>
@@ -2914,8 +3088,14 @@
         <f>VLOOKUP(A16,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>181</v>
+      </c>
+      <c r="K16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1421046</v>
       </c>
@@ -2944,8 +3124,14 @@
         <f>VLOOKUP(A17,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>173</v>
+      </c>
+      <c r="K17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1421046</v>
       </c>
@@ -2974,8 +3160,14 @@
         <f>VLOOKUP(A18,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>173</v>
+      </c>
+      <c r="K18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1421046</v>
       </c>
@@ -3004,8 +3196,14 @@
         <f>VLOOKUP(A19,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1421046</v>
       </c>
@@ -3031,8 +3229,14 @@
         <f>VLOOKUP(A20,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>179</v>
+      </c>
+      <c r="K20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1421046</v>
       </c>
@@ -3055,8 +3259,14 @@
         <f>VLOOKUP(A21,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:35</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>179</v>
+      </c>
+      <c r="K21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1421047</v>
       </c>
@@ -3085,8 +3295,14 @@
         <f>VLOOKUP(A22,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>173</v>
+      </c>
+      <c r="K22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1421047</v>
       </c>
@@ -3109,8 +3325,14 @@
         <f>VLOOKUP(A23,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>179</v>
+      </c>
+      <c r="K23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1421047</v>
       </c>
@@ -3133,8 +3355,14 @@
         <f>VLOOKUP(A24,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>179</v>
+      </c>
+      <c r="K24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1421047</v>
       </c>
@@ -3163,8 +3391,14 @@
         <f>VLOOKUP(A25,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>173</v>
+      </c>
+      <c r="K25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1421047</v>
       </c>
@@ -3193,8 +3427,14 @@
         <f>VLOOKUP(A26,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>173</v>
+      </c>
+      <c r="K26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1421047</v>
       </c>
@@ -3223,8 +3463,14 @@
         <f>VLOOKUP(A27,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>173</v>
+      </c>
+      <c r="K27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1421047</v>
       </c>
@@ -3253,8 +3499,14 @@
         <f>VLOOKUP(A28,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>173</v>
+      </c>
+      <c r="K28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1421047</v>
       </c>
@@ -3283,8 +3535,14 @@
         <f>VLOOKUP(A29,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>173</v>
+      </c>
+      <c r="K29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1421047</v>
       </c>
@@ -3313,8 +3571,14 @@
         <f>VLOOKUP(A30,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>173</v>
+      </c>
+      <c r="K30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1421047</v>
       </c>
@@ -3340,8 +3604,14 @@
         <f>VLOOKUP(A31,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>179</v>
+      </c>
+      <c r="K31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1421047</v>
       </c>
@@ -3370,8 +3640,14 @@
         <f>VLOOKUP(A32,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:31:56</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>173</v>
+      </c>
+      <c r="K32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1421048</v>
       </c>
@@ -3394,8 +3670,14 @@
         <f>VLOOKUP(A33,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>192</v>
+      </c>
+      <c r="K33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1421048</v>
       </c>
@@ -3418,8 +3700,14 @@
         <f>VLOOKUP(A34,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>179</v>
+      </c>
+      <c r="K34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1421048</v>
       </c>
@@ -3442,8 +3730,14 @@
         <f>VLOOKUP(A35,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>179</v>
+      </c>
+      <c r="K35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1421048</v>
       </c>
@@ -3466,8 +3760,14 @@
         <f>VLOOKUP(A36,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>192</v>
+      </c>
+      <c r="K36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1421048</v>
       </c>
@@ -3490,8 +3790,14 @@
         <f>VLOOKUP(A37,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>179</v>
+      </c>
+      <c r="K37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1421048</v>
       </c>
@@ -3514,8 +3820,14 @@
         <f>VLOOKUP(A38,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>179</v>
+      </c>
+      <c r="K38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1421048</v>
       </c>
@@ -3538,8 +3850,14 @@
         <f>VLOOKUP(A39,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>179</v>
+      </c>
+      <c r="K39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1421048</v>
       </c>
@@ -3562,8 +3880,14 @@
         <f>VLOOKUP(A40,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>179</v>
+      </c>
+      <c r="K40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1421048</v>
       </c>
@@ -3586,8 +3910,14 @@
         <f>VLOOKUP(A41,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>179</v>
+      </c>
+      <c r="K41" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1421048</v>
       </c>
@@ -3616,8 +3946,14 @@
         <f>VLOOKUP(A42,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" t="s">
+        <v>173</v>
+      </c>
+      <c r="K42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1421048</v>
       </c>
@@ -3646,8 +3982,14 @@
         <f>VLOOKUP(A43,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" t="s">
+        <v>173</v>
+      </c>
+      <c r="K43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1421048</v>
       </c>
@@ -3676,8 +4018,14 @@
         <f>VLOOKUP(A44,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" t="s">
+        <v>173</v>
+      </c>
+      <c r="K44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1421048</v>
       </c>
@@ -3706,8 +4054,14 @@
         <f>VLOOKUP(A45,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>173</v>
+      </c>
+      <c r="K45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1421048</v>
       </c>
@@ -3736,8 +4090,14 @@
         <f>VLOOKUP(A46,Usuarios!A:B,2,0)</f>
         <v>04/12/2024 09:32:13</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" t="s">
+        <v>181</v>
+      </c>
+      <c r="K46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1424749</v>
       </c>
@@ -3763,8 +4123,14 @@
         <f>VLOOKUP(A47,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" t="s">
+        <v>177</v>
+      </c>
+      <c r="K47" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1424749</v>
       </c>
@@ -3790,8 +4156,14 @@
         <f>VLOOKUP(A48,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" t="s">
+        <v>179</v>
+      </c>
+      <c r="K48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1424749</v>
       </c>
@@ -3814,8 +4186,14 @@
         <f>VLOOKUP(A49,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" t="s">
+        <v>179</v>
+      </c>
+      <c r="K49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1424749</v>
       </c>
@@ -3841,8 +4219,14 @@
         <f>VLOOKUP(A50,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" t="s">
+        <v>177</v>
+      </c>
+      <c r="K50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1424749</v>
       </c>
@@ -3865,8 +4249,14 @@
         <f>VLOOKUP(A51,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51" t="s">
+        <v>179</v>
+      </c>
+      <c r="K51" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1424749</v>
       </c>
@@ -3892,8 +4282,14 @@
         <f>VLOOKUP(A52,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52" t="s">
+        <v>179</v>
+      </c>
+      <c r="K52" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1424749</v>
       </c>
@@ -3916,8 +4312,14 @@
         <f>VLOOKUP(A53,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53" t="s">
+        <v>179</v>
+      </c>
+      <c r="K53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1424749</v>
       </c>
@@ -3940,8 +4342,14 @@
         <f>VLOOKUP(A54,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54" t="s">
+        <v>179</v>
+      </c>
+      <c r="K54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1424749</v>
       </c>
@@ -3964,8 +4372,14 @@
         <f>VLOOKUP(A55,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55" t="s">
+        <v>179</v>
+      </c>
+      <c r="K55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1424749</v>
       </c>
@@ -3991,8 +4405,14 @@
         <f>VLOOKUP(A56,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56" t="s">
+        <v>179</v>
+      </c>
+      <c r="K56" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1424749</v>
       </c>
@@ -4015,8 +4435,14 @@
         <f>VLOOKUP(A57,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57" t="s">
+        <v>179</v>
+      </c>
+      <c r="K57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1424749</v>
       </c>
@@ -4039,8 +4465,14 @@
         <f>VLOOKUP(A58,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58" t="s">
+        <v>179</v>
+      </c>
+      <c r="K58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1424749</v>
       </c>
@@ -4063,8 +4495,14 @@
         <f>VLOOKUP(A59,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59" t="s">
+        <v>179</v>
+      </c>
+      <c r="K59" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1424749</v>
       </c>
@@ -4087,8 +4525,14 @@
         <f>VLOOKUP(A60,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60" t="s">
+        <v>179</v>
+      </c>
+      <c r="K60" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1424749</v>
       </c>
@@ -4111,8 +4555,14 @@
         <f>VLOOKUP(A61,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61" t="s">
+        <v>179</v>
+      </c>
+      <c r="K61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1424749</v>
       </c>
@@ -4138,8 +4588,14 @@
         <f>VLOOKUP(A62,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62" t="s">
+        <v>179</v>
+      </c>
+      <c r="K62" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1424749</v>
       </c>
@@ -4168,8 +4624,14 @@
         <f>VLOOKUP(A63,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63" t="s">
+        <v>181</v>
+      </c>
+      <c r="K63" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1424749</v>
       </c>
@@ -4192,8 +4654,14 @@
         <f>VLOOKUP(A64,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64" t="s">
+        <v>179</v>
+      </c>
+      <c r="K64" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1424749</v>
       </c>
@@ -4219,8 +4687,14 @@
         <f>VLOOKUP(A65,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65" t="s">
+        <v>179</v>
+      </c>
+      <c r="K65" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1424749</v>
       </c>
@@ -4246,8 +4720,14 @@
         <f>VLOOKUP(A66,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 14:45:00</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66" t="s">
+        <v>179</v>
+      </c>
+      <c r="K66" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1424775</v>
       </c>
@@ -4270,8 +4750,14 @@
         <f>VLOOKUP(A67,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67" t="s">
+        <v>192</v>
+      </c>
+      <c r="K67" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1424775</v>
       </c>
@@ -4294,8 +4780,14 @@
         <f>VLOOKUP(A68,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68" t="s">
+        <v>179</v>
+      </c>
+      <c r="K68" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1424775</v>
       </c>
@@ -4318,8 +4810,14 @@
         <f>VLOOKUP(A69,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69" t="s">
+        <v>179</v>
+      </c>
+      <c r="K69" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1424775</v>
       </c>
@@ -4342,8 +4840,14 @@
         <f>VLOOKUP(A70,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70" t="s">
+        <v>192</v>
+      </c>
+      <c r="K70" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1424775</v>
       </c>
@@ -4366,8 +4870,14 @@
         <f>VLOOKUP(A71,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71" t="s">
+        <v>179</v>
+      </c>
+      <c r="K71" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1424775</v>
       </c>
@@ -4390,8 +4900,14 @@
         <f>VLOOKUP(A72,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72" t="s">
+        <v>179</v>
+      </c>
+      <c r="K72" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1424775</v>
       </c>
@@ -4414,8 +4930,14 @@
         <f>VLOOKUP(A73,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73" t="s">
+        <v>179</v>
+      </c>
+      <c r="K73" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1424775</v>
       </c>
@@ -4438,8 +4960,14 @@
         <f>VLOOKUP(A74,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J74" t="s">
+        <v>179</v>
+      </c>
+      <c r="K74" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1424775</v>
       </c>
@@ -4462,8 +4990,14 @@
         <f>VLOOKUP(A75,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75" t="s">
+        <v>179</v>
+      </c>
+      <c r="K75" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1424775</v>
       </c>
@@ -4486,8 +5020,14 @@
         <f>VLOOKUP(A76,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" t="s">
+        <v>179</v>
+      </c>
+      <c r="K76" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1424775</v>
       </c>
@@ -4510,8 +5050,14 @@
         <f>VLOOKUP(A77,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77" t="s">
+        <v>179</v>
+      </c>
+      <c r="K77" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1424775</v>
       </c>
@@ -4534,8 +5080,14 @@
         <f>VLOOKUP(A78,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78" t="s">
+        <v>179</v>
+      </c>
+      <c r="K78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1424775</v>
       </c>
@@ -4558,8 +5110,14 @@
         <f>VLOOKUP(A79,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79" t="s">
+        <v>179</v>
+      </c>
+      <c r="K79" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1424775</v>
       </c>
@@ -4581,6 +5139,12 @@
       <c r="I80" t="str">
         <f>VLOOKUP(A80,Usuarios!A:B,2,0)</f>
         <v>16/12/2024 15:45:08</v>
+      </c>
+      <c r="J80" t="s">
+        <v>179</v>
+      </c>
+      <c r="K80" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>